<commit_message>
Installed GitHub for Unity
</commit_message>
<xml_diff>
--- a/DesignDocuments/ScottsEscape_Phase1_M2_Statut.xlsx
+++ b/DesignDocuments/ScottsEscape_Phase1_M2_Statut.xlsx
@@ -47,9 +47,6 @@
     <t>Vidéo de présentation</t>
   </si>
   <si>
-    <t>Résultats de playtest</t>
-  </si>
-  <si>
     <t>Build du jeu</t>
   </si>
   <si>
@@ -78,6 +75,9 @@
   </si>
   <si>
     <t>Racine du répertoire drive</t>
+  </si>
+  <si>
+    <t>Résultats de playtests</t>
   </si>
 </sst>
 </file>
@@ -468,7 +468,7 @@
   <dimension ref="A1:D39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -476,7 +476,7 @@
     <col min="1" max="1" width="21" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="20.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="24.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="46.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="51.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -490,7 +490,7 @@
         <v>2</v>
       </c>
       <c r="D1" s="9" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -501,10 +501,10 @@
         <v>0.9</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -515,10 +515,10 @@
         <v>0.9</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -529,7 +529,7 @@
         <v>1</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D4" s="6"/>
     </row>
@@ -541,55 +541,55 @@
         <v>1</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D5" s="6"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="B6" s="8">
         <v>1</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D6" s="6"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B7" s="8">
         <v>1</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D7" s="6"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B8" s="8">
         <v>0.25</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D8" s="6"/>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B9" s="8">
         <v>1</v>
       </c>
       <c r="C9" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D9" s="6"/>
     </row>

</xml_diff>